<commit_message>
Revert "Merge branch 'pj/at/release_ver4' into pj/at/teamb/dakoku6"
This reverts commit 599933e897137408a4c3327540f77dbe367daf6e, reversing
changes made to 17de5ed761f874972ee0c5a3ba1d6edc28fc33da.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UKclone\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UK-teamA\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12456"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト（出力イメージ）" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>【会社】</t>
     <rPh sb="1" eb="3">
@@ -586,6 +586,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>外出応援区分</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>外出区分</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -634,6 +638,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>&amp;=item.outSupportAtr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>&amp;=item.outAtr</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -643,63 +651,6 @@
   </si>
   <si>
     <t>&amp;=item.empInfoTerMemo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.workplaceCode</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.workplaceName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_出勤</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_退勤</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_外出</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_戻り</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampAttendance</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampLeaveWork</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampGoingout</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampReturn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>職場コード（応援時）</t>
-    <rPh sb="0" eb="2">
-      <t>ショクバ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>オウエン</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>職場（応援時）</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2767,10 +2718,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
@@ -3460,7 +3411,7 @@
       <sheetName val="選択肢管理"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -3881,13 +3832,13 @@
             <v>保守委託</v>
           </cell>
           <cell r="AK4" t="str">
-            <v>保守委託</v>
+            <v>保守支援</v>
           </cell>
           <cell r="AL4" t="str">
             <v>保守料金</v>
           </cell>
           <cell r="AM4" t="str">
-            <v>保守支援</v>
+            <v>保守委託</v>
           </cell>
           <cell r="AN4" t="str">
             <v>保守支援</v>
@@ -39858,7 +39809,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -40041,7 +39992,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45360,17 +45311,17 @@
       <sheetName val="内示書"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45447,8 +45398,6 @@
       <sheetName val="別紙３（全体概要ﾌﾛｰ1）"/>
       <sheetName val="別紙３（全体概要ﾌﾛｰ2）"/>
       <sheetName val="データ授受一覧"/>
-      <sheetName val="参照シート"/>
-      <sheetName val="table詳細"/>
     </sheetNames>
     <definedNames>
       <definedName name="ワイドに"/>
@@ -45522,8 +45471,6 @@
       <sheetData sheetId="64"/>
       <sheetData sheetId="65"/>
       <sheetData sheetId="66"/>
-      <sheetData sheetId="67" refreshError="1"/>
-      <sheetData sheetId="68" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45800,7 +45747,7 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -46101,26 +46048,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="1"/>
-    <col min="7" max="8" width="10.6640625" style="2"/>
-    <col min="9" max="19" width="10.6640625" style="1"/>
-    <col min="20" max="20" width="15.33203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="1"/>
+    <col min="2" max="3" width="10.625" style="1"/>
+    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.625" style="1"/>
+    <col min="7" max="8" width="10.625" style="2"/>
+    <col min="9" max="20" width="10.625" style="1"/>
+    <col min="21" max="21" width="15.375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.375" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -46128,7 +46075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -46136,7 +46083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -46144,7 +46091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -46152,17 +46099,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -46182,96 +46129,66 @@
         <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="36">
+    <row r="11" spans="1:13" ht="24">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
+      <c r="G11" s="5" t="s">
+        <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
+      <c r="I11" s="6" t="s">
+        <v>31</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>22</v>
+      <c r="J11" s="5" t="s">
+        <v>32</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>23</v>
+      <c r="K11" s="5" t="s">
+        <v>33</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="M11" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R11" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'pj/at/release_ver4' into pj/at/teamb/dakoku6""
This reverts commit 70a449c45a1e72665db69a4ffe9fa7a4da9cc91b.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UK-teamA\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UKclone\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト（出力イメージ）" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>【会社】</t>
     <rPh sb="1" eb="3">
@@ -586,10 +586,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>外出応援区分</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>外出区分</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -638,10 +634,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&amp;=item.outSupportAtr</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&amp;=item.outAtr</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -651,6 +643,63 @@
   </si>
   <si>
     <t>&amp;=item.empInfoTerMemo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.workplaceCode</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.workplaceName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_出勤</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_退勤</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_外出</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_戻り</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampAttendance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampLeaveWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampGoingout</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampReturn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>職場コード（応援時）</t>
+    <rPh sb="0" eb="2">
+      <t>ショクバ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>オウエン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>職場（応援時）</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2718,10 +2767,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
@@ -3411,7 +3460,7 @@
       <sheetName val="選択肢管理"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -3832,13 +3881,13 @@
             <v>保守委託</v>
           </cell>
           <cell r="AK4" t="str">
-            <v>保守支援</v>
+            <v>保守委託</v>
           </cell>
           <cell r="AL4" t="str">
             <v>保守料金</v>
           </cell>
           <cell r="AM4" t="str">
-            <v>保守委託</v>
+            <v>保守支援</v>
           </cell>
           <cell r="AN4" t="str">
             <v>保守支援</v>
@@ -39809,7 +39858,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -39992,7 +40041,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45311,17 +45360,17 @@
       <sheetName val="内示書"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45398,6 +45447,8 @@
       <sheetName val="別紙３（全体概要ﾌﾛｰ1）"/>
       <sheetName val="別紙３（全体概要ﾌﾛｰ2）"/>
       <sheetName val="データ授受一覧"/>
+      <sheetName val="参照シート"/>
+      <sheetName val="table詳細"/>
     </sheetNames>
     <definedNames>
       <definedName name="ワイドに"/>
@@ -45471,6 +45522,8 @@
       <sheetData sheetId="64"/>
       <sheetData sheetId="65"/>
       <sheetData sheetId="66"/>
+      <sheetData sheetId="67" refreshError="1"/>
+      <sheetData sheetId="68" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45747,7 +45800,7 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -46048,26 +46101,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.625" style="1"/>
-    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.625" style="1"/>
-    <col min="7" max="8" width="10.625" style="2"/>
-    <col min="9" max="20" width="10.625" style="1"/>
-    <col min="21" max="21" width="15.375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="12.375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.625" style="1"/>
+    <col min="2" max="3" width="10.6640625" style="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" style="1"/>
+    <col min="7" max="8" width="10.6640625" style="2"/>
+    <col min="9" max="19" width="10.6640625" style="1"/>
+    <col min="20" max="20" width="15.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -46075,7 +46128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -46083,7 +46136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -46091,7 +46144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -46099,17 +46152,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:18">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -46129,66 +46182,96 @@
         <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="L10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="4" t="s">
+    </row>
+    <row r="11" spans="1:18" ht="36">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="24">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
+      <c r="G11" s="5" t="s">
+        <v>34</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>27</v>
+      <c r="H11" s="5" t="s">
+        <v>35</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="K11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="L11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="Q11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="R11" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'origin/uk/release_pj/sinsei7_1051' into uk/release_bug/main"
This reverts commit 2146204050fb0899c07495d4e79ab7bc8366c523, reversing
changes made to 8275455b37a55a0a47c042061349e007f6ebf715.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UKclone\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UK-teamA\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12456"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト（出力イメージ）" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>【会社】</t>
     <rPh sb="1" eb="3">
@@ -586,6 +586,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>外出応援区分</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>外出区分</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -634,6 +638,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>&amp;=item.outSupportAtr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>&amp;=item.outAtr</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -643,63 +651,6 @@
   </si>
   <si>
     <t>&amp;=item.empInfoTerMemo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.workplaceCode</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.workplaceName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_出勤</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_退勤</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_外出</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打刻変換_戻り</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampAttendance</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampLeaveWork</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampGoingout</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&amp;=item.stampReturn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>職場コード（応援時）</t>
-    <rPh sb="0" eb="2">
-      <t>ショクバ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>オウエン</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>職場（応援時）</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2767,10 +2718,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
@@ -3460,7 +3411,7 @@
       <sheetName val="選択肢管理"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -3881,13 +3832,13 @@
             <v>保守委託</v>
           </cell>
           <cell r="AK4" t="str">
-            <v>保守委託</v>
+            <v>保守支援</v>
           </cell>
           <cell r="AL4" t="str">
             <v>保守料金</v>
           </cell>
           <cell r="AM4" t="str">
-            <v>保守支援</v>
+            <v>保守委託</v>
           </cell>
           <cell r="AN4" t="str">
             <v>保守支援</v>
@@ -39858,7 +39809,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -40041,7 +39992,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45360,17 +45311,17 @@
       <sheetName val="内示書"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45447,8 +45398,6 @@
       <sheetName val="別紙３（全体概要ﾌﾛｰ1）"/>
       <sheetName val="別紙３（全体概要ﾌﾛｰ2）"/>
       <sheetName val="データ授受一覧"/>
-      <sheetName val="参照シート"/>
-      <sheetName val="table詳細"/>
     </sheetNames>
     <definedNames>
       <definedName name="ワイドに"/>
@@ -45522,8 +45471,6 @@
       <sheetData sheetId="64"/>
       <sheetData sheetId="65"/>
       <sheetData sheetId="66"/>
-      <sheetData sheetId="67" refreshError="1"/>
-      <sheetData sheetId="68" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45800,7 +45747,7 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -46101,26 +46048,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="1"/>
-    <col min="7" max="8" width="10.6640625" style="2"/>
-    <col min="9" max="19" width="10.6640625" style="1"/>
-    <col min="20" max="20" width="15.33203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="1"/>
+    <col min="2" max="3" width="10.625" style="1"/>
+    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.625" style="1"/>
+    <col min="7" max="8" width="10.625" style="2"/>
+    <col min="9" max="20" width="10.625" style="1"/>
+    <col min="21" max="21" width="15.375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.375" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -46128,7 +46075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -46136,7 +46083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -46144,7 +46091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -46152,17 +46099,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -46182,96 +46129,66 @@
         <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="36">
+    <row r="11" spans="1:13" ht="24">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
+      <c r="G11" s="5" t="s">
+        <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
+      <c r="I11" s="6" t="s">
+        <v>31</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>22</v>
+      <c r="J11" s="5" t="s">
+        <v>32</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>23</v>
+      <c r="K11" s="5" t="s">
+        <v>33</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="M11" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R11" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge remote-tracking branch 'origin/uk/release_pj/sinsei7_1051' into uk/release_bug/main""
This reverts commit f8f6e19801e7c5094cc46fbbad38a35d5959947f.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UK-teamA\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UKclone\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト（出力イメージ）" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>【会社】</t>
     <rPh sb="1" eb="3">
@@ -586,10 +586,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>外出応援区分</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>外出区分</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -638,10 +634,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&amp;=item.outSupportAtr</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&amp;=item.outAtr</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -651,6 +643,63 @@
   </si>
   <si>
     <t>&amp;=item.empInfoTerMemo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.workplaceCode</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.workplaceName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_出勤</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_退勤</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_外出</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打刻変換_戻り</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampAttendance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampLeaveWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampGoingout</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=item.stampReturn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>職場コード（応援時）</t>
+    <rPh sb="0" eb="2">
+      <t>ショクバ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>オウエン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>職場（応援時）</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2718,10 +2767,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
@@ -3411,7 +3460,7 @@
       <sheetName val="選択肢管理"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -3832,13 +3881,13 @@
             <v>保守委託</v>
           </cell>
           <cell r="AK4" t="str">
-            <v>保守支援</v>
+            <v>保守委託</v>
           </cell>
           <cell r="AL4" t="str">
             <v>保守料金</v>
           </cell>
           <cell r="AM4" t="str">
-            <v>保守委託</v>
+            <v>保守支援</v>
           </cell>
           <cell r="AN4" t="str">
             <v>保守支援</v>
@@ -39809,7 +39858,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -39992,7 +40041,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45311,17 +45360,17 @@
       <sheetName val="内示書"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45398,6 +45447,8 @@
       <sheetName val="別紙３（全体概要ﾌﾛｰ1）"/>
       <sheetName val="別紙３（全体概要ﾌﾛｰ2）"/>
       <sheetName val="データ授受一覧"/>
+      <sheetName val="参照シート"/>
+      <sheetName val="table詳細"/>
     </sheetNames>
     <definedNames>
       <definedName name="ワイドに"/>
@@ -45471,6 +45522,8 @@
       <sheetData sheetId="64"/>
       <sheetData sheetId="65"/>
       <sheetData sheetId="66"/>
+      <sheetData sheetId="67" refreshError="1"/>
+      <sheetData sheetId="68" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45747,7 +45800,7 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
@@ -46048,26 +46101,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.625" style="1"/>
-    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.625" style="1"/>
-    <col min="7" max="8" width="10.625" style="2"/>
-    <col min="9" max="20" width="10.625" style="1"/>
-    <col min="21" max="21" width="15.375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="12.375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.625" style="1"/>
+    <col min="2" max="3" width="10.6640625" style="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" style="1"/>
+    <col min="7" max="8" width="10.6640625" style="2"/>
+    <col min="9" max="19" width="10.6640625" style="1"/>
+    <col min="20" max="20" width="15.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -46075,7 +46128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -46083,7 +46136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -46091,7 +46144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -46099,17 +46152,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:18">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -46129,66 +46182,96 @@
         <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="L10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="4" t="s">
+    </row>
+    <row r="11" spans="1:18" ht="36">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="24">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
+      <c r="G11" s="5" t="s">
+        <v>34</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>27</v>
+      <c r="H11" s="5" t="s">
+        <v>35</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="K11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="L11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="Q11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="R11" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KNR001: Init commit code
# Conflicts:
#	nts.uk/uk.at/at.web/nts.uk.at.web/src/main/webapp/view/knr/001/a/knr001.a.vm.ts
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UKclone\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12456"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト（出力イメージ）" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
@@ -50,46 +50,48 @@
     <externalReference r:id="rId34"/>
     <externalReference r:id="rId35"/>
     <externalReference r:id="rId36"/>
+    <externalReference r:id="rId37"/>
   </externalReferences>
   <definedNames>
+    <definedName name="\RE">[1]MASTER!#REF!</definedName>
     <definedName name="_">#REF!</definedName>
     <definedName name="___">#REF!</definedName>
     <definedName name="____">#REF!</definedName>
-    <definedName name="______a1">[1]!______a1</definedName>
-    <definedName name="______a2">[1]!______a2</definedName>
-    <definedName name="______a3">[1]!______a3</definedName>
-    <definedName name="______a4">[1]!______a4</definedName>
-    <definedName name="____a1">[1]!____a1</definedName>
-    <definedName name="____a2">[1]!____a2</definedName>
-    <definedName name="____a3">[1]!____a3</definedName>
-    <definedName name="____a4">[1]!____a4</definedName>
-    <definedName name="____HON1">[2]WBS!#REF!</definedName>
-    <definedName name="____HON2">[2]WBS!#REF!</definedName>
-    <definedName name="____KYO1">[2]WBS!#REF!</definedName>
-    <definedName name="___HON1">[2]WBS!#REF!</definedName>
-    <definedName name="___HON2">[2]WBS!#REF!</definedName>
-    <definedName name="___KYO1">[2]WBS!#REF!</definedName>
+    <definedName name="______a1">[2]!______a1</definedName>
+    <definedName name="______a2">[2]!______a2</definedName>
+    <definedName name="______a3">[2]!______a3</definedName>
+    <definedName name="______a4">[2]!______a4</definedName>
+    <definedName name="____a1">[2]!____a1</definedName>
+    <definedName name="____a2">[2]!____a2</definedName>
+    <definedName name="____a3">[2]!____a3</definedName>
+    <definedName name="____a4">[2]!____a4</definedName>
+    <definedName name="____HON1">[3]WBS!#REF!</definedName>
+    <definedName name="____HON2">[3]WBS!#REF!</definedName>
+    <definedName name="____KYO1">[3]WBS!#REF!</definedName>
+    <definedName name="___HON1">[3]WBS!#REF!</definedName>
+    <definedName name="___HON2">[3]WBS!#REF!</definedName>
+    <definedName name="___KYO1">[3]WBS!#REF!</definedName>
     <definedName name="___sss1" hidden="1">#REF!</definedName>
-    <definedName name="__a1">[1]!__a1</definedName>
-    <definedName name="__a2">[1]!__a2</definedName>
-    <definedName name="__a3">[1]!__a3</definedName>
-    <definedName name="__a4">[1]!__a4</definedName>
+    <definedName name="__a1">[2]!__a1</definedName>
+    <definedName name="__a2">[2]!__a2</definedName>
+    <definedName name="__a3">[2]!__a3</definedName>
+    <definedName name="__a4">[2]!__a4</definedName>
     <definedName name="__sss1" hidden="1">#REF!</definedName>
-    <definedName name="_12_0GRAD_">[3]工数0511!#REF!</definedName>
-    <definedName name="_16GRAD_">[4]工数0511!#REF!</definedName>
+    <definedName name="_12_0GRAD_">[4]工数0511!#REF!</definedName>
+    <definedName name="_16GRAD_">[5]工数0511!#REF!</definedName>
     <definedName name="_20_0">#REF!</definedName>
-    <definedName name="_24_0">[5]SHEET1!#REF!</definedName>
+    <definedName name="_24_0">[6]SHEET1!#REF!</definedName>
     <definedName name="_28_0_0WEEK">#REF!</definedName>
     <definedName name="_32_0AR">#REF!</definedName>
-    <definedName name="_35a1_">[1]!_35a1_</definedName>
-    <definedName name="_38a2_">[1]!_38a2_</definedName>
+    <definedName name="_35a1_">[2]!_35a1_</definedName>
+    <definedName name="_38a2_">[2]!_38a2_</definedName>
     <definedName name="_4_">#REF!</definedName>
-    <definedName name="_41a3_">[1]!_41a3_</definedName>
-    <definedName name="_44a4_">[1]!_44a4_</definedName>
+    <definedName name="_41a3_">[2]!_41a3_</definedName>
+    <definedName name="_44a4_">[2]!_44a4_</definedName>
     <definedName name="_48AR">#REF!</definedName>
     <definedName name="_52WEEK">#REF!</definedName>
-    <definedName name="_8_">[5]SHEET1!#REF!</definedName>
-    <definedName name="_ETC" hidden="1">'[6]テーブル定義書（案件番号採番）'!#REF!</definedName>
+    <definedName name="_8_">[6]SHEET1!#REF!</definedName>
+    <definedName name="_ETC" hidden="1">[7]テーブル定義書（案件番号採番）!#REF!</definedName>
     <definedName name="_FFILL" hidden="1">#REF!</definedName>
     <definedName name="_Fil" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
@@ -97,10 +99,10 @@
     <definedName name="_FILL2" hidden="1">#REF!</definedName>
     <definedName name="_filla" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" hidden="1">#REF!</definedName>
-    <definedName name="_HON1">[2]WBS!#REF!</definedName>
-    <definedName name="_HON2">[2]WBS!#REF!</definedName>
+    <definedName name="_HON1">[3]WBS!#REF!</definedName>
+    <definedName name="_HON2">[3]WBS!#REF!</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
-    <definedName name="_KYO1">[2]WBS!#REF!</definedName>
+    <definedName name="_KYO1">[3]WBS!#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
     <definedName name="_Parse_In" hidden="1">#REF!</definedName>
@@ -112,9 +114,8 @@
     <definedName name="_sss1" hidden="1">#REF!</definedName>
     <definedName name="_take" hidden="1">#REF!</definedName>
     <definedName name="_面接から採用に至るまでの情報管理とする_____アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う_">#REF!</definedName>
-    <definedName name="\RE">[7]MASTER!#REF!</definedName>
     <definedName name="・面接から採用に至るまでの情報管理とする。___・アウトソーシングにて_採用された情報を_ファイ__ルにて取込を行う。">#REF!</definedName>
-    <definedName name="a">'[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="a">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="A1Width">#REF!</definedName>
     <definedName name="AA" hidden="1">#REF!</definedName>
     <definedName name="AAA">#REF!</definedName>
@@ -136,8 +137,8 @@
     <definedName name="ｂｂｂｂ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="bbbbb" hidden="1">#REF!</definedName>
     <definedName name="BSTART">[9]OLD!#REF!</definedName>
+    <definedName name="B列">#REF!</definedName>
     <definedName name="Ｂ自入金比率">[10]基礎数字!$C$51</definedName>
-    <definedName name="B列">#REF!</definedName>
     <definedName name="cal_index_size">[11]!cal_index_size</definedName>
     <definedName name="cal_table_size">[11]!cal_table_size</definedName>
     <definedName name="ccc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -145,9 +146,9 @@
     <definedName name="ｃde" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="column_def_array">{"区分",0,"Auto","Auto",""}</definedName>
     <definedName name="CULC.cal_index_size">[12]!CULC.cal_index_size</definedName>
+    <definedName name="C保守単価">'[13]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価">'[13]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守支援単価">'[13]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価">'[13]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C列">#REF!</definedName>
     <definedName name="d">{"区分",0,"Auto","Auto",""}</definedName>
     <definedName name="_xlnm.Database">[14]PR!#REF!</definedName>
@@ -162,22 +163,22 @@
     <definedName name="DS_NM">#REF!</definedName>
     <definedName name="D列">#REF!</definedName>
     <definedName name="e" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
-    <definedName name="EIGY1">[2]WBS!$C$41,[2]WBS!#REF!</definedName>
-    <definedName name="EIGY2">[2]WBS!#REF!</definedName>
-    <definedName name="EIGY3">[2]WBS!#REF!</definedName>
-    <definedName name="EIGY4">[2]WBS!#REF!</definedName>
-    <definedName name="EIGY5">[2]WBS!#REF!</definedName>
+    <definedName name="EIGY1">[3]WBS!$C$41,[3]WBS!#REF!</definedName>
+    <definedName name="EIGY2">[3]WBS!#REF!</definedName>
+    <definedName name="EIGY3">[3]WBS!#REF!</definedName>
+    <definedName name="EIGY4">[3]WBS!#REF!</definedName>
+    <definedName name="EIGY5">[3]WBS!#REF!</definedName>
     <definedName name="ENDM">#REF!</definedName>
     <definedName name="E列">#REF!</definedName>
-    <definedName name="f">[1]!f</definedName>
+    <definedName name="f">[2]!f</definedName>
     <definedName name="Filll" hidden="1">#REF!</definedName>
     <definedName name="F列">#REF!</definedName>
-    <definedName name="g">[1]!g</definedName>
+    <definedName name="g">[2]!g</definedName>
     <definedName name="GRAD_TAB">'[15]基礎(ADSG)'!#REF!</definedName>
     <definedName name="G列">#REF!</definedName>
     <definedName name="h">{"入社Y",0,"Auto","Auto",""}</definedName>
     <definedName name="ｈｈｈ">#REF!</definedName>
-    <definedName name="HONN">[2]WBS!#REF!</definedName>
+    <definedName name="HONN">[3]WBS!#REF!</definedName>
     <definedName name="HTML_CodePage" hidden="1">932</definedName>
     <definedName name="HTML_Control" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="HTML_Control_2" hidden="1">{"'Sheet1'!$A$1:$O$49"}</definedName>
@@ -212,34 +213,34 @@
     <definedName name="kosuke">[17]工数見積!#REF!</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ＬＨ">#REF!</definedName>
-    <definedName name="LIB">[2]WBS!#REF!</definedName>
+    <definedName name="LIB">[3]WBS!#REF!</definedName>
     <definedName name="lo" hidden="1">{"'Sheet1'!$A$1:$O$49"}</definedName>
     <definedName name="ＬサＨ">#REF!</definedName>
     <definedName name="Ｌサホ">#REF!</definedName>
     <definedName name="ＬニＨ">#REF!</definedName>
     <definedName name="Ｌニホ">#REF!</definedName>
     <definedName name="Ｌホ">#REF!</definedName>
-    <definedName name="MAST">[2]WBS!#REF!</definedName>
+    <definedName name="MAST">[3]WBS!#REF!</definedName>
     <definedName name="ＭＨ">#REF!</definedName>
     <definedName name="Ｍホ">#REF!</definedName>
-    <definedName name="ｎ">'[18]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="ｎ">[18]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="NAMES">#REF!</definedName>
-    <definedName name="NAYO">[2]WBS!#REF!</definedName>
+    <definedName name="NAYO">[3]WBS!#REF!</definedName>
     <definedName name="NEC_KEYS">#REF!</definedName>
-    <definedName name="NETW">[2]WBS!#REF!</definedName>
+    <definedName name="NETW">[3]WBS!#REF!</definedName>
     <definedName name="ＯＨ">#REF!</definedName>
     <definedName name="OPT_NO">[19]!OPT_NO</definedName>
     <definedName name="OPT_YES">[19]!OPT_YES</definedName>
-    <definedName name="OSCH">[2]WBS!#REF!</definedName>
+    <definedName name="OSCH">[3]WBS!#REF!</definedName>
     <definedName name="Ｏホ">#REF!</definedName>
     <definedName name="PARTS1">#REF!</definedName>
     <definedName name="PG単価">[20]明細合計!#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="PIV更新">[1]!PIV更新</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'マスタリスト（出力イメージ）'!$A$1:$M$11</definedName>
+    <definedName name="PIV更新">[2]!PIV更新</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト（出力イメージ）!$A$1:$M$11</definedName>
     <definedName name="PrintDaicho">[21]!PrintDaicho</definedName>
     <definedName name="QuitDaicho">[21]!QuitDaicho</definedName>
-    <definedName name="Record1">[1]!Record1</definedName>
+    <definedName name="Record1">[2]!Record1</definedName>
     <definedName name="row_def_array">{"入社Y",0,"Auto","Auto",""}</definedName>
     <definedName name="SE単価">[20]明細合計!#REF!</definedName>
     <definedName name="sisann" hidden="1">#REF!</definedName>
@@ -254,13 +255,13 @@
     <definedName name="TBL_KEYS">#REF!</definedName>
     <definedName name="TBL_KEYS2">#REF!</definedName>
     <definedName name="T列">#REF!</definedName>
-    <definedName name="UNN">[2]WBS!#REF!</definedName>
+    <definedName name="UNN">[3]WBS!#REF!</definedName>
     <definedName name="U列">#REF!</definedName>
     <definedName name="value_def_array">{"名前","COUNT(名前)","YNNNN",FALSE}</definedName>
     <definedName name="Ver002001006特休残管理対応" hidden="1">#REF!</definedName>
     <definedName name="V列">#REF!</definedName>
     <definedName name="ｗ">'[13]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="WBS">[2]WBS!#REF!</definedName>
+    <definedName name="WBS">[3]WBS!#REF!</definedName>
     <definedName name="WC単価">'[13]見積明細(ハードのみ）'!$X$5:$X$34</definedName>
     <definedName name="WD">[22]MASTER!#REF!</definedName>
     <definedName name="WEEKDAY">[22]MASTER!#REF!</definedName>
@@ -268,7 +269,7 @@
     <definedName name="wrn.PRINT_ALL." hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="wrn.REPORT1." hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="W列">#REF!</definedName>
-    <definedName name="X">[1]!X</definedName>
+    <definedName name="X">[2]!X</definedName>
     <definedName name="ＸＸＸ" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="X列">#REF!</definedName>
     <definedName name="Y列">#REF!</definedName>
@@ -282,15 +283,15 @@
     <definedName name="ああああああああああ">#REF!</definedName>
     <definedName name="あい" hidden="1">#REF!</definedName>
     <definedName name="あいう" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
-    <definedName name="ｱﾗｰﾑﾁｪｯｸ2">[3]工数0511!#REF!</definedName>
+    <definedName name="ｱﾗｰﾑﾁｪｯｸ2">[4]工数0511!#REF!</definedName>
     <definedName name="い" hidden="1">#REF!</definedName>
     <definedName name="え" hidden="1">#REF!</definedName>
     <definedName name="えらー" hidden="1">[23]表紙!#REF!</definedName>
     <definedName name="エラー一覧" hidden="1">[23]表紙!#REF!</definedName>
-    <definedName name="オーダー№">[1]!オーダー№</definedName>
+    <definedName name="オーダー№">[2]!オーダー№</definedName>
     <definedName name="オブジェクトの定義">#REF!</definedName>
+    <definedName name="カード入金比率">[10]基礎数字!$C$48</definedName>
     <definedName name="カード種類利用件数">[10]基礎数字!$C$59</definedName>
-    <definedName name="カード入金比率">[10]基礎数字!$C$48</definedName>
     <definedName name="クＨ">#REF!</definedName>
     <definedName name="クサＨ">#REF!</definedName>
     <definedName name="クサホ">#REF!</definedName>
@@ -298,8 +299,8 @@
     <definedName name="クニホ">#REF!</definedName>
     <definedName name="クホ">#REF!</definedName>
     <definedName name="こおおｋ">#REF!</definedName>
-    <definedName name="サＨ">'[24]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
-    <definedName name="サホ">'[24]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ'!#REF!</definedName>
+    <definedName name="サＨ">[24]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
+    <definedName name="サホ">[24]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName name="サホ1">#REF!</definedName>
     <definedName name="ｻﾎﾟｰﾄﾏﾆｭｱﾙ" hidden="1">#REF!</definedName>
     <definedName name="サンプル" hidden="1">#REF!</definedName>
@@ -309,7 +310,7 @@
     <definedName name="ステータス数">[10]基礎数字!$C$23</definedName>
     <definedName name="だ" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="タスクドキュメント１" hidden="1">#REF!</definedName>
-    <definedName name="ち">[1]!ち</definedName>
+    <definedName name="ち">[2]!ち</definedName>
     <definedName name="チャネル共通率">[10]基礎数字!$C$6</definedName>
     <definedName name="ｯb" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="ツール別見積工数">#REF!</definedName>
@@ -335,10 +336,84 @@
     <definedName name="ワイドに">[27]!ワイドに</definedName>
     <definedName name="んんんん" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ">#REF!</definedName>
-    <definedName name="印刷">[28]!印刷</definedName>
+    <definedName name="予定">[28]進捗入力ｼｰﾄ!#REF!</definedName>
+    <definedName name="人日原価">#REF!</definedName>
+    <definedName name="仕切り">'[13]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="仕切単価">'[13]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="代引入金比率">[10]基礎数字!$C$49</definedName>
+    <definedName name="仮顧客保存月数">[10]基礎数字!$C$9</definedName>
     <definedName name="仮顧客発生数">[10]基礎数字!$C$8</definedName>
-    <definedName name="仮顧客保存月数">[10]基礎数字!$C$9</definedName>
+    <definedName name="会員数">[10]基礎数字!$C$29</definedName>
+    <definedName name="会社共通率">[10]基礎数字!$C$4</definedName>
+    <definedName name="住民税115">#REF!</definedName>
+    <definedName name="住民税96">#REF!</definedName>
+    <definedName name="住民税納付先の登録7">#REF!</definedName>
     <definedName name="価格表">#REF!</definedName>
+    <definedName name="保守単価">'[13]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
+    <definedName name="保守委託単価">'[13]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
+    <definedName name="保守支援単価">'[13]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
+    <definedName name="値引単価">'[13]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
+    <definedName name="備考">'[13]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
+    <definedName name="債権">[2]!債権</definedName>
+    <definedName name="入出荷ファイル保管月数">[10]基礎数字!$C$73</definedName>
+    <definedName name="入出荷件数">[10]基礎数字!$C$72</definedName>
+    <definedName name="入金ファイル保管月数">[10]基礎数字!$C$52</definedName>
+    <definedName name="入金分割率">[10]基礎数字!$C$60</definedName>
+    <definedName name="入金振替件数">[10]基礎数字!$C$61</definedName>
+    <definedName name="入金経路対外会社数">[10]基礎数字!$C$58</definedName>
+    <definedName name="共通更新">[2]!共通更新</definedName>
+    <definedName name="処理サイクル" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
+    <definedName name="出荷件数">[10]基礎数字!$C$22</definedName>
+    <definedName name="出荷保管月数">[10]基礎数字!$C$18</definedName>
+    <definedName name="削除０１" hidden="1">[7]テーブル定義書（案件番号採番）!#REF!</definedName>
+    <definedName name="削除０２" hidden="1">#REF!</definedName>
+    <definedName name="削除０３" hidden="1">#REF!</definedName>
+    <definedName name="削除０４" hidden="1">[7]テーブル定義書（案件番号採番）!#REF!</definedName>
+    <definedName name="削除０５" hidden="1">#REF!</definedName>
+    <definedName name="削除０６" hidden="1">#REF!</definedName>
+    <definedName name="削除０７" hidden="1">[7]テーブル定義書（案件番号採番）!#REF!</definedName>
+    <definedName name="削除０８" hidden="1">#REF!</definedName>
+    <definedName name="削除０９" hidden="1">#REF!</definedName>
+    <definedName name="単価">#REF!</definedName>
+    <definedName name="単価種別">#REF!</definedName>
+    <definedName name="印刷">[29]!印刷</definedName>
+    <definedName name="原価">#REF!</definedName>
+    <definedName name="受注エラー履歴保管月数">[10]基礎数字!$C$25</definedName>
+    <definedName name="受注エラー率">[10]基礎数字!$C$24</definedName>
+    <definedName name="受注保管月数">[10]基礎数字!$C$17</definedName>
+    <definedName name="受注数">[10]基礎数字!$C$15</definedName>
+    <definedName name="受注明細数">[10]基礎数字!$C$16</definedName>
+    <definedName name="口座変更率">[10]基礎数字!$C$12</definedName>
+    <definedName name="口座登録率">[10]基礎数字!$C$11</definedName>
+    <definedName name="商品数">[10]基礎数字!$C$43</definedName>
+    <definedName name="商品群共通率">[10]基礎数字!$C$5</definedName>
+    <definedName name="問合せ件数">[10]基礎数字!$C$36</definedName>
+    <definedName name="売上">[2]!売上</definedName>
+    <definedName name="売値">#REF!</definedName>
+    <definedName name="定価">#REF!</definedName>
+    <definedName name="定期購入者数">[10]基礎数字!$C$80</definedName>
+    <definedName name="定期購入者明細申込み数">[10]基礎数字!$C$81</definedName>
+    <definedName name="宿泊">#REF!</definedName>
+    <definedName name="宿泊単金">#REF!</definedName>
+    <definedName name="届け先違い率">[10]基礎数字!$C$19</definedName>
+    <definedName name="工程別生産性">#REF!</definedName>
+    <definedName name="平均購入商品">[10]基礎数字!$C$26</definedName>
+    <definedName name="店舗DF_KEYS">#REF!</definedName>
+    <definedName name="店舗売上件数">[10]基礎数字!$C$30</definedName>
+    <definedName name="店舗売上保管月数">[10]基礎数字!$C$32</definedName>
+    <definedName name="店舗売上明細数">[10]基礎数字!$C$31</definedName>
+    <definedName name="払込入金比率">[10]基礎数字!$C$47</definedName>
+    <definedName name="日帰り">#REF!</definedName>
+    <definedName name="日帰り単金">#REF!</definedName>
+    <definedName name="未顧客相談率">[10]基礎数字!$C$69</definedName>
+    <definedName name="検討項目Sample2">[2]!検討項目Sample2</definedName>
+    <definedName name="検討項目一覧Sample">[2]!検討項目一覧Sample</definedName>
+    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
+    <definedName name="標準価格">'[13]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
+    <definedName name="機種SORT">[30]!機種SORT</definedName>
+    <definedName name="機能別原価">#REF!</definedName>
+    <definedName name="物流DF_KEYS">#REF!</definedName>
+    <definedName name="生産性TBL">[31]２－２．支援明細AS400!#REF!</definedName>
     <definedName name="画面1">#REF!</definedName>
     <definedName name="画面2">#REF!</definedName>
     <definedName name="画面３">#REF!</definedName>
@@ -346,29 +421,37 @@
     <definedName name="画面5">#REF!</definedName>
     <definedName name="画面6">#REF!</definedName>
     <definedName name="画面7">#REF!</definedName>
-    <definedName name="会員数">[10]基礎数字!$C$29</definedName>
-    <definedName name="会社共通率">[10]基礎数字!$C$4</definedName>
+    <definedName name="番号">[32]型TB!#REF!</definedName>
+    <definedName name="直扱単価">'[13]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
+    <definedName name="相談件数">[10]基礎数字!$C$66</definedName>
+    <definedName name="相談保管月数">[10]基礎数字!$C$67</definedName>
+    <definedName name="相談明細件数">[10]基礎数字!$C$68</definedName>
+    <definedName name="督促レベルＡ比率">[10]基礎数字!$C$53</definedName>
+    <definedName name="督促レベルＥ比率">[10]基礎数字!$C$57</definedName>
+    <definedName name="督促停止率">[10]基礎数字!$C$62</definedName>
+    <definedName name="社共単価">'[13]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
+    <definedName name="種別">#REF!</definedName>
+    <definedName name="終了">[33]!終了</definedName>
+    <definedName name="見やすく">[27]!見やすく</definedName>
+    <definedName name="見積工数">#REF!</definedName>
     <definedName name="解析">#N/A</definedName>
-    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
-    <definedName name="関連表" hidden="1">#REF!</definedName>
-    <definedName name="関連表２" hidden="1">#REF!</definedName>
-    <definedName name="機種SORT">[29]!機種SORT</definedName>
-    <definedName name="機能別原価">#REF!</definedName>
-    <definedName name="共通更新">[1]!共通更新</definedName>
+    <definedName name="設計書">#N/A</definedName>
+    <definedName name="請求分割率">[10]基礎数字!$C$21</definedName>
+    <definedName name="返戻種類追加" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
+    <definedName name="返戻種類追加２" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
+    <definedName name="返金予約率">[10]基礎数字!$C$40</definedName>
+    <definedName name="返金率">[10]基礎数字!$C$39</definedName>
+    <definedName name="部">'[13]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
+    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
+    <definedName name="郵自入金比率">[10]基礎数字!$C$50</definedName>
+    <definedName name="重複" hidden="1">[34]表紙!#REF!</definedName>
     <definedName name="銀行の登録48">#REF!</definedName>
     <definedName name="銀行の登録67">#REF!</definedName>
     <definedName name="銀行の登録7">#REF!</definedName>
-    <definedName name="検討項目Sample2">[1]!検討項目Sample2</definedName>
-    <definedName name="検討項目一覧Sample">[1]!検討項目一覧Sample</definedName>
-    <definedName name="見やすく">[27]!見やすく</definedName>
-    <definedName name="見積工数">#REF!</definedName>
-    <definedName name="原価">#REF!</definedName>
-    <definedName name="顧客メモ発生率">[10]基礎数字!$C$10</definedName>
-    <definedName name="顧客数">[10]基礎数字!$C$3</definedName>
-    <definedName name="顧客変更率">[10]基礎数字!$C$7</definedName>
-    <definedName name="口座登録率">[10]基礎数字!$C$11</definedName>
-    <definedName name="口座変更率">[10]基礎数字!$C$12</definedName>
-    <definedName name="工程別生産性">#REF!</definedName>
+    <definedName name="関連表" hidden="1">#REF!</definedName>
+    <definedName name="関連表２" hidden="1">#REF!</definedName>
+    <definedName name="電子帳票仕様" hidden="1">[35]表紙!#REF!</definedName>
+    <definedName name="電車">#REF!</definedName>
     <definedName name="項目名の登録1">#REF!</definedName>
     <definedName name="項目名の登録2">#REF!</definedName>
     <definedName name="項目名の登録3">#REF!</definedName>
@@ -377,92 +460,10 @@
     <definedName name="項目名の登録6">#REF!</definedName>
     <definedName name="項目名の登録7">#REF!</definedName>
     <definedName name="項目名の登録8">#REF!</definedName>
-    <definedName name="債権">[1]!債権</definedName>
-    <definedName name="削除０１" hidden="1">'[6]テーブル定義書（案件番号採番）'!#REF!</definedName>
-    <definedName name="削除０２" hidden="1">#REF!</definedName>
-    <definedName name="削除０３" hidden="1">#REF!</definedName>
-    <definedName name="削除０４" hidden="1">'[6]テーブル定義書（案件番号採番）'!#REF!</definedName>
-    <definedName name="削除０５" hidden="1">#REF!</definedName>
-    <definedName name="削除０６" hidden="1">#REF!</definedName>
-    <definedName name="削除０７" hidden="1">'[6]テーブル定義書（案件番号採番）'!#REF!</definedName>
-    <definedName name="削除０８" hidden="1">#REF!</definedName>
-    <definedName name="削除０９" hidden="1">#REF!</definedName>
-    <definedName name="仕切り">'[13]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="仕切単価">'[13]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="社共単価">'[13]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
-    <definedName name="種別">#REF!</definedName>
-    <definedName name="受注エラー履歴保管月数">[10]基礎数字!$C$25</definedName>
-    <definedName name="受注エラー率">[10]基礎数字!$C$24</definedName>
-    <definedName name="受注数">[10]基礎数字!$C$15</definedName>
-    <definedName name="受注保管月数">[10]基礎数字!$C$17</definedName>
-    <definedName name="受注明細数">[10]基礎数字!$C$16</definedName>
-    <definedName name="終了">[30]!終了</definedName>
-    <definedName name="住民税115">#REF!</definedName>
-    <definedName name="住民税96">#REF!</definedName>
-    <definedName name="住民税納付先の登録7">#REF!</definedName>
-    <definedName name="重複" hidden="1">[31]表紙!#REF!</definedName>
-    <definedName name="宿泊">#REF!</definedName>
-    <definedName name="宿泊単金">#REF!</definedName>
-    <definedName name="出荷件数">[10]基礎数字!$C$22</definedName>
-    <definedName name="出荷保管月数">[10]基礎数字!$C$18</definedName>
-    <definedName name="処理サイクル" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
-    <definedName name="商品群共通率">[10]基礎数字!$C$5</definedName>
-    <definedName name="商品数">[10]基礎数字!$C$43</definedName>
-    <definedName name="人日原価">#REF!</definedName>
-    <definedName name="生産性TBL">'[32]２－２．支援明細AS400'!#REF!</definedName>
-    <definedName name="請求分割率">[10]基礎数字!$C$21</definedName>
-    <definedName name="設計書">#N/A</definedName>
-    <definedName name="相談件数">[10]基礎数字!$C$66</definedName>
-    <definedName name="相談保管月数">[10]基礎数字!$C$67</definedName>
-    <definedName name="相談明細件数">[10]基礎数字!$C$68</definedName>
-    <definedName name="代引入金比率">[10]基礎数字!$C$49</definedName>
-    <definedName name="単価">#REF!</definedName>
-    <definedName name="単価種別">#REF!</definedName>
-    <definedName name="値引単価">'[13]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
-    <definedName name="直扱単価">'[13]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
-    <definedName name="定価">#REF!</definedName>
-    <definedName name="定期購入者数">[10]基礎数字!$C$80</definedName>
-    <definedName name="定期購入者明細申込み数">[10]基礎数字!$C$81</definedName>
-    <definedName name="店舗DF_KEYS">#REF!</definedName>
-    <definedName name="店舗売上件数">[10]基礎数字!$C$30</definedName>
-    <definedName name="店舗売上保管月数">[10]基礎数字!$C$32</definedName>
-    <definedName name="店舗売上明細数">[10]基礎数字!$C$31</definedName>
-    <definedName name="電子帳票仕様" hidden="1">[33]表紙!#REF!</definedName>
-    <definedName name="電車">#REF!</definedName>
-    <definedName name="督促レベルＡ比率">[10]基礎数字!$C$53</definedName>
-    <definedName name="督促レベルＥ比率">[10]基礎数字!$C$57</definedName>
-    <definedName name="督促停止率">[10]基礎数字!$C$62</definedName>
-    <definedName name="届け先違い率">[10]基礎数字!$C$19</definedName>
-    <definedName name="日帰り">#REF!</definedName>
-    <definedName name="日帰り単金">#REF!</definedName>
-    <definedName name="入金ファイル保管月数">[10]基礎数字!$C$52</definedName>
-    <definedName name="入金経路対外会社数">[10]基礎数字!$C$58</definedName>
-    <definedName name="入金振替件数">[10]基礎数字!$C$61</definedName>
-    <definedName name="入金分割率">[10]基礎数字!$C$60</definedName>
-    <definedName name="入出荷ファイル保管月数">[10]基礎数字!$C$73</definedName>
-    <definedName name="入出荷件数">[10]基礎数字!$C$72</definedName>
-    <definedName name="売上">[1]!売上</definedName>
-    <definedName name="売値">#REF!</definedName>
-    <definedName name="番号">[34]型TB!#REF!</definedName>
+    <definedName name="顧客メモ発生率">[10]基礎数字!$C$10</definedName>
+    <definedName name="顧客変更率">[10]基礎数字!$C$7</definedName>
+    <definedName name="顧客数">[10]基礎数字!$C$3</definedName>
     <definedName name="飛行機">#REF!</definedName>
-    <definedName name="備考">'[13]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
-    <definedName name="標準価格">'[13]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
-    <definedName name="部">'[13]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
-    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
-    <definedName name="払込入金比率">[10]基礎数字!$C$47</definedName>
-    <definedName name="物流DF_KEYS">#REF!</definedName>
-    <definedName name="平均購入商品">[10]基礎数字!$C$26</definedName>
-    <definedName name="返金予約率">[10]基礎数字!$C$40</definedName>
-    <definedName name="返金率">[10]基礎数字!$C$39</definedName>
-    <definedName name="返戻種類追加" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
-    <definedName name="返戻種類追加２" hidden="1">{"'Sheet1'!$A$1:$I$153"}</definedName>
-    <definedName name="保守委託単価">'[13]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
-    <definedName name="保守支援単価">'[13]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
-    <definedName name="保守単価">'[13]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
-    <definedName name="未顧客相談率">[10]基礎数字!$C$69</definedName>
-    <definedName name="問合せ件数">[10]基礎数字!$C$36</definedName>
-    <definedName name="郵自入金比率">[10]基礎数字!$C$50</definedName>
-    <definedName name="予定">[35]進捗入力ｼｰﾄ!#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -474,7 +475,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>【会社】</t>
     <rPh sb="1" eb="3">
@@ -702,22 +703,118 @@
     <t>職場（応援時）</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>項目</t>
+  </si>
+  <si>
+    <t>内容</t>
+  </si>
+  <si>
+    <t>設定値</t>
+  </si>
+  <si>
+    <t>申告の利用</t>
+  </si>
+  <si>
+    <t>申告枠の設定</t>
+  </si>
+  <si>
+    <t>深夜残業の自動計算</t>
+  </si>
+  <si>
+    <t>申告時間反映先</t>
+  </si>
+  <si>
+    <t>早出残業</t>
+  </si>
+  <si>
+    <t>普通残業</t>
+  </si>
+  <si>
+    <t>法内休出</t>
+  </si>
+  <si>
+    <t>法外休出</t>
+  </si>
+  <si>
+    <t>法外祝日</t>
+  </si>
+  <si>
+    <t>早出残業深夜</t>
+  </si>
+  <si>
+    <t>普通残業深夜</t>
+  </si>
+  <si>
+    <t>法内休出深夜</t>
+  </si>
+  <si>
+    <t>法外休出深夜</t>
+  </si>
+  <si>
+    <t>法外祝日深夜</t>
+  </si>
+  <si>
+    <t>&amp;=usageAtr</t>
+  </si>
+  <si>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.usageAtr</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.frameSet</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.midnightAutoCalc</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.earlyOvertime</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.earlyOvertimeMn</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.overtime</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.overtimeMn</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.statutory</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.notStatutory</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.notStatHoliday</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.statutoryMn</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.notStatutoryMn</t>
+  </si>
+  <si>
+    <t>&amp;=declareSet.notStatHolidayMn</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -740,6 +837,12 @@
       <name val="MS Gothic"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -784,7 +887,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -803,13 +906,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -825,72 +962,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="表紙"/>
-      <sheetName val="修正履歴"/>
-      <sheetName val="画面遷移図"/>
-      <sheetName val="画面状態遷移図"/>
-      <sheetName val="画面イメージ"/>
-      <sheetName val="画面イメージ＿部品（製品版）"/>
-      <sheetName val="項目定義"/>
-      <sheetName val="処理概要"/>
-      <sheetName val="項目制御"/>
-      <sheetName val="項目移送表"/>
-      <sheetName val="多言語参照"/>
-      <sheetName val="補足資料"/>
-      <sheetName val="画面部品"/>
-      <sheetName val="画面部品 (2)"/>
-      <sheetName val="ボツ画面"/>
-      <sheetName val="ボツ"/>
-      <sheetName val="画面設計書-KTG031-トップページアラーム"/>
+      <sheetName val="MASTER"/>
     </sheetNames>
-    <definedNames>
-      <definedName name="______a1" refersTo="#REF!"/>
-      <definedName name="______a2" refersTo="#REF!"/>
-      <definedName name="______a3" refersTo="#REF!"/>
-      <definedName name="______a4" refersTo="#REF!"/>
-      <definedName name="____a1" refersTo="#REF!"/>
-      <definedName name="____a2" refersTo="#REF!"/>
-      <definedName name="____a3" refersTo="#REF!"/>
-      <definedName name="____a4" refersTo="#REF!"/>
-      <definedName name="__a1" refersTo="#REF!"/>
-      <definedName name="__a2" refersTo="#REF!"/>
-      <definedName name="__a3" refersTo="#REF!"/>
-      <definedName name="__a4" refersTo="#REF!"/>
-      <definedName name="_35a1_" refersTo="#REF!"/>
-      <definedName name="_38a2_" refersTo="#REF!"/>
-      <definedName name="_41a3_" refersTo="#REF!"/>
-      <definedName name="_44a4_" refersTo="#REF!"/>
-      <definedName name="f" refersTo="#REF!"/>
-      <definedName name="g" refersTo="#REF!"/>
-      <definedName name="PIV更新" refersTo="#REF!"/>
-      <definedName name="Record1" refersTo="#REF!"/>
-      <definedName name="X" refersTo="#REF!"/>
-      <definedName name="オーダー№" refersTo="#REF!"/>
-      <definedName name="ち" refersTo="#REF!"/>
-      <definedName name="共通更新" refersTo="#REF!"/>
-      <definedName name="検討項目Sample2" refersTo="#REF!"/>
-      <definedName name="検討項目一覧Sample" refersTo="#REF!"/>
-      <definedName name="債権" refersTo="#REF!"/>
-      <definedName name="売上" refersTo="#REF!"/>
-    </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1305,6 +1380,8 @@
       <sheetName val="費用比較 "/>
       <sheetName val="ﾊｰﾄﾞ明細(FT1200）"/>
       <sheetName val="master"/>
+      <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
+      <sheetName val="工数0511"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
@@ -2773,6 +2850,8 @@
       <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3474,6 +3553,7 @@
     <sheetNames>
       <sheetName val="仕切価格"/>
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
+      <sheetName val="テーブル定義書（案件番号採番）"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
@@ -3652,7 +3732,7 @@
             <v>型番</v>
           </cell>
           <cell r="D2" t="str">
-            <v xml:space="preserve">製品名 </v>
+            <v>製品名</v>
           </cell>
           <cell r="E2" t="str">
             <v>仕様</v>
@@ -25233,7 +25313,7 @@
             <v>ACW-CD-S</v>
           </cell>
           <cell r="C140" t="str">
-            <v xml:space="preserve">M6754-5 </v>
+            <v>M6754-5</v>
           </cell>
           <cell r="D140" t="str">
             <v>内蔵CD-ROM装置</v>
@@ -39825,6 +39905,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -39887,40 +39968,72 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="WBS"/>
-      <sheetName val="工数"/>
-      <sheetName val="工数 (2)"/>
-      <sheetName val="SCHEDULE1"/>
-      <sheetName val="PARTS"/>
-      <sheetName val="記入要領"/>
-      <sheetName val="SUB DELETE"/>
-      <sheetName val="MAIN LINE"/>
-      <sheetName val="Module2"/>
-      <sheetName val="STATUS"/>
-      <sheetName val="前提"/>
-      <sheetName val="Module1"/>
-      <sheetName val="Module3"/>
+      <sheetName val="表紙"/>
+      <sheetName val="修正履歴"/>
+      <sheetName val="画面遷移図"/>
+      <sheetName val="画面状態遷移図"/>
+      <sheetName val="画面イメージ"/>
+      <sheetName val="画面イメージ＿部品（製品版）"/>
+      <sheetName val="項目定義"/>
+      <sheetName val="処理概要"/>
+      <sheetName val="項目制御"/>
+      <sheetName val="項目移送表"/>
+      <sheetName val="多言語参照"/>
+      <sheetName val="補足資料"/>
+      <sheetName val="画面部品"/>
+      <sheetName val="画面部品 (2)"/>
+      <sheetName val="ボツ画面"/>
+      <sheetName val="ボツ"/>
+      <sheetName val="画面設計書-KTG031-トップページアラーム"/>
     </sheetNames>
+    <definedNames>
+      <definedName name="______a1" refersTo="#REF!"/>
+      <definedName name="______a2" refersTo="#REF!"/>
+      <definedName name="______a3" refersTo="#REF!"/>
+      <definedName name="______a4" refersTo="#REF!"/>
+      <definedName name="____a1" refersTo="#REF!"/>
+      <definedName name="____a2" refersTo="#REF!"/>
+      <definedName name="____a3" refersTo="#REF!"/>
+      <definedName name="____a4" refersTo="#REF!"/>
+      <definedName name="__a1" refersTo="#REF!"/>
+      <definedName name="__a2" refersTo="#REF!"/>
+      <definedName name="__a3" refersTo="#REF!"/>
+      <definedName name="__a4" refersTo="#REF!"/>
+      <definedName name="_35a1_" refersTo="#REF!"/>
+      <definedName name="_38a2_" refersTo="#REF!"/>
+      <definedName name="_41a3_" refersTo="#REF!"/>
+      <definedName name="_44a4_" refersTo="#REF!"/>
+      <definedName name="f" refersTo="#REF!"/>
+      <definedName name="g" refersTo="#REF!"/>
+      <definedName name="PIV更新" refersTo="#REF!"/>
+      <definedName name="Record1" refersTo="#REF!"/>
+      <definedName name="X" refersTo="#REF!"/>
+      <definedName name="オーダー№" refersTo="#REF!"/>
+      <definedName name="ち" refersTo="#REF!"/>
+      <definedName name="共通更新" refersTo="#REF!"/>
+      <definedName name="検討項目Sample2" refersTo="#REF!"/>
+      <definedName name="検討項目一覧Sample" refersTo="#REF!"/>
+      <definedName name="債権" refersTo="#REF!"/>
+      <definedName name="売上" refersTo="#REF!"/>
+    </definedNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1">
-        <row r="41">
-          <cell r="C41" t="str">
-            <v>統合ﾃｽﾄ環境準備</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -40055,6 +40168,7 @@
       <sheetName val="テーブル設計991127"/>
       <sheetName val="仕切価格"/>
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
+      <sheetName val="sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
@@ -42545,7 +42659,7 @@
             <v>1</v>
           </cell>
           <cell r="E170" t="str">
-            <v xml:space="preserve">'0':未処理、'1':仮処理、'2':本処理、'3':出力不要 </v>
+            <v>'0':未処理、'1':仮処理、'2':本処理、'3':出力不要</v>
           </cell>
         </row>
         <row r="171">
@@ -45338,6 +45452,7 @@
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45533,6 +45648,37 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="WORK SHEET"/>
+      <sheetName val="集計macro"/>
+      <sheetName val="README"/>
+      <sheetName val="進捗入力ｼｰﾄ"/>
+      <sheetName val="進捗管理表"/>
+      <sheetName val="工数積上ｸﾞﾗﾌ"/>
+      <sheetName val="進捗率ｸﾞﾗﾌ"/>
+      <sheetName val="計算WORK(1)"/>
+      <sheetName val="計算WORK(2)"/>
+      <sheetName val="要件定義ｽｹｼﾞｭｰﾙ案"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="COPYFAN"/>
     </sheetNames>
     <definedNames>
@@ -45545,7 +45691,50 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="WBS"/>
+      <sheetName val="工数"/>
+      <sheetName val="工数 (2)"/>
+      <sheetName val="SCHEDULE1"/>
+      <sheetName val="PARTS"/>
+      <sheetName val="記入要領"/>
+      <sheetName val="SUB DELETE"/>
+      <sheetName val="MAIN LINE"/>
+      <sheetName val="Module2"/>
+      <sheetName val="STATUS"/>
+      <sheetName val="前提"/>
+      <sheetName val="Module1"/>
+      <sheetName val="Module3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1">
+        <row r="41">
+          <cell r="C41" t="str">
+            <v>統合ﾃｽﾄ環境準備</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -45563,20 +45752,61 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="工数0511"/>
+      <sheetName val="２－１．支援対象本数サマリー"/>
+      <sheetName val="２－２．支援明細AS400"/>
+      <sheetName val="２－３．支援明細POS"/>
+      <sheetName val="2．ご支援内容"/>
+      <sheetName val="貴社作業"/>
+      <sheetName val="４．スケジュール"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="変更履歴"/>
+      <sheetName val="DS"/>
+      <sheetName val="MAC"/>
+      <sheetName val="T-ID"/>
+      <sheetName val="DD"/>
+      <sheetName val="型TB"/>
+      <sheetName val="DD(Webあり)"/>
+      <sheetName val="検索"/>
+      <sheetName val="MAC印"/>
+      <sheetName val="MAC店"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -45592,7 +45822,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink34.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -45619,30 +45849,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="２－１．支援対象本数サマリー"/>
-      <sheetName val="２－２．支援明細AS400"/>
-      <sheetName val="２－３．支援明細POS"/>
-      <sheetName val="2．ご支援内容"/>
-      <sheetName val="貴社作業"/>
-      <sheetName val="４．スケジュール"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink35.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -45675,68 +45882,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink34.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="変更履歴"/>
-      <sheetName val="DS"/>
-      <sheetName val="MAC"/>
-      <sheetName val="T-ID"/>
-      <sheetName val="DD"/>
-      <sheetName val="型TB"/>
-      <sheetName val="DD(Webあり)"/>
-      <sheetName val="検索"/>
-      <sheetName val="MAC印"/>
-      <sheetName val="MAC店"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink35.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="WORK SHEET"/>
-      <sheetName val="集計macro"/>
-      <sheetName val="README"/>
-      <sheetName val="進捗入力ｼｰﾄ"/>
-      <sheetName val="進捗管理表"/>
-      <sheetName val="工数積上ｸﾞﾗﾌ"/>
-      <sheetName val="進捗率ｸﾞﾗﾌ"/>
-      <sheetName val="計算WORK(1)"/>
-      <sheetName val="計算WORK(2)"/>
-      <sheetName val="要件定義ｽｹｼﾞｭｰﾙ案"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -45754,7 +45899,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="SHEET1"/>
+      <sheetName val="工数0511"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -45767,12 +45912,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="テーブル定義書（案件番号採番）"/>
-      <sheetName val="案件採番ﾃｰﾌﾞﾙ"/>
+      <sheetName val="SHEET1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45782,10 +45925,12 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="MASTER"/>
+      <sheetName val="テーブル定義書（案件番号採番）"/>
+      <sheetName val="案件採番ﾃｰﾌﾞﾙ"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -45836,7 +45981,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -46101,23 +46246,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" style="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="1"/>
-    <col min="7" max="8" width="10.6640625" style="2"/>
-    <col min="9" max="19" width="10.6640625" style="1"/>
-    <col min="20" max="20" width="15.33203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="1"/>
+    <col min="2" max="3" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="1"/>
+    <col min="7" max="8" width="10.7109375" style="2"/>
+    <col min="9" max="19" width="10.7109375" style="1"/>
+    <col min="20" max="20" width="15.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -46160,6 +46305,11 @@
     <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -46274,9 +46424,212 @@
         <v>33</v>
       </c>
     </row>
+    <row r="17" spans="3:4">
+      <c r="D17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.62" bottom="0.37" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToWidth="3" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="22" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
KNR001: - Update file xlsx
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46445,8 +46445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -46607,7 +46607,7 @@
       <c r="B21" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="11" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KNR001: Change file excel
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KNR001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46446,7 +46446,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -46554,7 +46554,7 @@
         <v>54</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -46590,7 +46590,7 @@
         <v>58</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3">

</xml_diff>